<commit_message>
numeric and radio button add
</commit_message>
<xml_diff>
--- a/media/uploads/Jononi Scripts.xlsx
+++ b/media/uploads/Jononi Scripts.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ur_sensei/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atique.hossain\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1CE844-B884-B945-BFC2-56807BC3DFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1589A18D-AC32-4337-9E93-E237A040177E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M Advocacy Meeting" sheetId="2" r:id="rId1"/>
     <sheet name="M QIC Meeting" sheetId="3" r:id="rId2"/>
-    <sheet name="MPerformanceReviewMeeting" sheetId="4" r:id="rId3"/>
+    <sheet name="M_Performance_Review_Meeting" sheetId="4" r:id="rId3"/>
     <sheet name="S Awareness Session" sheetId="5" r:id="rId4"/>
     <sheet name="S Community Dialogue Session" sheetId="6" r:id="rId5"/>
     <sheet name="S Folk Song, Video Show" sheetId="7" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="157">
   <si>
     <t>Question SR</t>
   </si>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t>Approximate Female listened</t>
+  </si>
+  <si>
+    <t>pdf</t>
   </si>
 </sst>
 </file>
@@ -951,15 +954,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="32.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1303,18 +1306,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,22 +1541,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B12DE93-9028-4403-99E2-D68D9B18F6DB}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1806,22 +1809,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F04D4EF-010A-49FB-8FE1-D0D1DA187F02}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2247,20 +2250,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692573CB-E0BF-4A48-8191-88DD9AE7F0C1}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2712,18 +2717,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3013,18 +3018,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>